<commit_message>
uploaded numerical model and graphs
</commit_message>
<xml_diff>
--- a/reading flight data/eigenvalues_of_all_motions.xlsx
+++ b/reading flight data/eigenvalues_of_all_motions.xlsx
@@ -9,17 +9,17 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView minimized="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Type of Motion</t>
   </si>
@@ -58,36 +58,6 @@
   </si>
   <si>
     <t>Roll Damping</t>
-  </si>
-  <si>
-    <t>short period 1</t>
-  </si>
-  <si>
-    <t>short period 2</t>
-  </si>
-  <si>
-    <t>phugoid</t>
-  </si>
-  <si>
-    <t>spiral</t>
-  </si>
-  <si>
-    <t>dutch roll</t>
-  </si>
-  <si>
-    <t>roll damping</t>
-  </si>
-  <si>
-    <t>V kts</t>
-  </si>
-  <si>
-    <t>V m/s</t>
-  </si>
-  <si>
-    <t>mac/b</t>
-  </si>
-  <si>
-    <t>(mac/b)/V</t>
   </si>
 </sst>
 </file>
@@ -455,21 +425,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J17"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" customWidth="1"/>
-    <col min="4" max="4" width="21.7109375" customWidth="1"/>
-    <col min="6" max="6" width="21.85546875" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -486,7 +457,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -494,27 +465,19 @@
         <v>5</v>
       </c>
       <c r="C2">
-        <v>0.61638616386163858</v>
+        <v>0.52751252751252742</v>
       </c>
       <c r="D2">
-        <v>-2.2708167358062491E-2</v>
+        <v>-1.313991885327281</v>
       </c>
       <c r="E2">
-        <v>2.541496219221262</v>
+        <v>2.139967007664378</v>
       </c>
       <c r="F2">
-        <v>4.9922911691530868E-2</v>
-      </c>
-      <c r="H2">
-        <f>D2/E12</f>
-        <v>-1.1245339710700211</v>
-      </c>
-      <c r="J2">
-        <f>F2/E12</f>
-        <v>2.4722386992591363</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+        <v>2.936113166547011</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -522,27 +485,19 @@
         <v>6</v>
       </c>
       <c r="C3">
-        <v>0.65415654156541581</v>
+        <v>0.5946730946730947</v>
       </c>
       <c r="D3">
-        <v>-2.647881142360493E-2</v>
+        <v>-1.1655936459358129</v>
       </c>
       <c r="E3">
-        <v>3.3831109100921659</v>
+        <v>3.9776852954326332</v>
       </c>
       <c r="F3">
-        <v>4.641072438264935E-2</v>
-      </c>
-      <c r="H3">
-        <f>D3/E13</f>
-        <v>-1.0596044471270192</v>
-      </c>
-      <c r="J3">
-        <f>F3/E13</f>
-        <v>1.8572212008882716</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+        <v>1.579608450772674</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -550,27 +505,19 @@
         <v>7</v>
       </c>
       <c r="C4">
-        <v>303.59828598285981</v>
+        <v>293.22031822031818</v>
       </c>
       <c r="D4">
-        <v>-5.7053311910351602E-5</v>
+        <v>-2.3639125172735549E-3</v>
       </c>
       <c r="E4">
-        <v>39.440317584217709</v>
+        <v>39.453345113869858</v>
       </c>
       <c r="F4">
-        <v>3.9810183492805119E-3</v>
-      </c>
-      <c r="H4">
-        <f>D4/E14</f>
-        <v>-2.2831063697081552E-3</v>
-      </c>
-      <c r="J4">
-        <f>F4/E14</f>
-        <v>0.15930868948412935</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+        <v>0.15925608561314941</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -578,17 +525,13 @@
         <v>8</v>
       </c>
       <c r="C5">
-        <v>20.831758317583169</v>
+        <v>55.030955030955027</v>
       </c>
       <c r="D5">
-        <v>-6.3524830167618158E-3</v>
-      </c>
-      <c r="H5">
-        <f>D5/E15</f>
-        <v>-3.3273580174693666E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+        <v>-1.259558697773005E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -596,17 +539,13 @@
         <v>9</v>
       </c>
       <c r="C6">
-        <v>10.625206252062521</v>
+        <v>22.074322074322069</v>
       </c>
       <c r="D6">
-        <v>-1.245466561141303E-2</v>
-      </c>
-      <c r="H6">
-        <f>D6/E16</f>
-        <v>-6.4833423268981005E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+        <v>-3.140061009466958E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -614,27 +553,19 @@
         <v>10</v>
       </c>
       <c r="C7">
-        <v>2.8750037500375001</v>
+        <v>3.2740532740532742</v>
       </c>
       <c r="D7">
-        <v>-4.6314839571065303E-2</v>
+        <v>-0.21170919424344919</v>
       </c>
       <c r="E7">
-        <v>3.3781403128261962</v>
+        <v>3.388627376855152</v>
       </c>
       <c r="F7">
-        <v>0.35730188105857102</v>
-      </c>
-      <c r="H7">
-        <f>D7/E16</f>
-        <v>-0.24109435702506618</v>
-      </c>
-      <c r="J7">
-        <f>F7/E16</f>
-        <v>1.8599539170482209</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+        <v>1.854197764585954</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -642,27 +573,19 @@
         <v>11</v>
       </c>
       <c r="C8">
-        <v>2.9855548555485552</v>
+        <v>2.9177054177054171</v>
       </c>
       <c r="D8">
-        <v>-4.4599862970775152E-2</v>
+        <v>-0.2375658544394999</v>
       </c>
       <c r="E8">
-        <v>3.3799083516346911</v>
+        <v>3.3977451840740009</v>
       </c>
       <c r="F8">
-        <v>0.35711497551962218</v>
-      </c>
-      <c r="H8">
-        <f>D8/E16</f>
-        <v>-0.23216695525515268</v>
-      </c>
-      <c r="J8">
-        <f>F8/E16</f>
-        <v>1.8589809703392477</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+        <v>1.8492220477951951</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -670,142 +593,10 @@
         <v>12</v>
       </c>
       <c r="C9">
-        <v>0.37754627546275449</v>
+        <v>0.64507939507939493</v>
       </c>
       <c r="D9">
-        <v>-0.31722049198024121</v>
-      </c>
-      <c r="H9">
-        <f>D9/E17</f>
-        <v>-1.8359264164647424</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>19</v>
-      </c>
-      <c r="C11" t="s">
-        <v>20</v>
-      </c>
-      <c r="D11" t="s">
-        <v>21</v>
-      </c>
-      <c r="E11" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12">
-        <v>198</v>
-      </c>
-      <c r="C12">
-        <f>B12*0.514444444</f>
-        <v>101.85999991200001</v>
-      </c>
-      <c r="D12">
-        <v>2.0569000000000002</v>
-      </c>
-      <c r="E12">
-        <f>D12/C12</f>
-        <v>2.019340272704712E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>14</v>
-      </c>
-      <c r="B13">
-        <v>160</v>
-      </c>
-      <c r="C13">
-        <f t="shared" ref="C13:C17" si="0">B13*0.514444444</f>
-        <v>82.31111104</v>
-      </c>
-      <c r="D13">
-        <v>2.0569000000000002</v>
-      </c>
-      <c r="E13">
-        <f t="shared" ref="E13:E17" si="1">D13/C13</f>
-        <v>2.4989335874720811E-2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>15</v>
-      </c>
-      <c r="B14">
-        <v>160</v>
-      </c>
-      <c r="C14">
-        <f t="shared" si="0"/>
-        <v>82.31111104</v>
-      </c>
-      <c r="D14">
-        <v>2.0569000000000002</v>
-      </c>
-      <c r="E14">
-        <f t="shared" si="1"/>
-        <v>2.4989335874720811E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>16</v>
-      </c>
-      <c r="B15">
-        <v>162</v>
-      </c>
-      <c r="C15">
-        <f t="shared" si="0"/>
-        <v>83.339999927999997</v>
-      </c>
-      <c r="D15">
-        <v>15.911</v>
-      </c>
-      <c r="E15">
-        <f t="shared" si="1"/>
-        <v>0.19091672682680591</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>17</v>
-      </c>
-      <c r="B16">
-        <v>161</v>
-      </c>
-      <c r="C16">
-        <f t="shared" si="0"/>
-        <v>82.825555484000006</v>
-      </c>
-      <c r="D16">
-        <v>15.911</v>
-      </c>
-      <c r="E16">
-        <f t="shared" si="1"/>
-        <v>0.19210254500585439</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>18</v>
-      </c>
-      <c r="B17">
-        <v>179</v>
-      </c>
-      <c r="C17">
-        <f t="shared" si="0"/>
-        <v>92.085555475999996</v>
-      </c>
-      <c r="D17">
-        <v>15.911</v>
-      </c>
-      <c r="E17">
-        <f t="shared" si="1"/>
-        <v>0.17278497064772377</v>
+        <v>-1.07451452619198</v>
       </c>
     </row>
   </sheetData>

</xml_diff>